<commit_message>
Table one code improved, sample size calculation, visualization with labels in axis.
</commit_message>
<xml_diff>
--- a/results/statistics/hypothesis_testing.xlsx
+++ b/results/statistics/hypothesis_testing.xlsx
@@ -712,7 +712,7 @@
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H7">
         <v>0.0004768904387608621</v>
@@ -840,7 +840,7 @@
         <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H11">
         <v>0.001111123112164218</v>
@@ -1000,7 +1000,7 @@
         <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H16">
         <v>0.1782239131206481</v>

</xml_diff>